<commit_message>
i am adding more LDC right now
</commit_message>
<xml_diff>
--- a/elder_paper_02_severn.xlsx
+++ b/elder_paper_02_severn.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Initial Concentration" sheetId="10" r:id="rId3"/>
     <sheet name="Loading" sheetId="3" r:id="rId4"/>
     <sheet name="hidden tab" sheetId="11" r:id="rId5"/>
-    <sheet name="LDC" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="LDC" sheetId="12" r:id="rId6"/>
     <sheet name="چاتا" sheetId="14" state="hidden" r:id="rId7"/>
     <sheet name="ماکیناو" sheetId="15" state="hidden" r:id="rId8"/>
     <sheet name="سورن سفارش نوری" sheetId="13" state="hidden" r:id="rId9"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="115">
   <si>
     <t>Project Name</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>St1 @ 0.21 (km)</t>
+  </si>
+  <si>
+    <t>1.0e+03 *</t>
   </si>
 </sst>
 </file>
@@ -4686,7 +4689,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4964,7 +4967,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="51">
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -7347,7 +7350,7 @@
       </c>
       <c r="AB2" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7359,7 +7362,7 @@
       </c>
       <c r="AE2" s="75">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF2" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7491,7 +7494,7 @@
       </c>
       <c r="AB3" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7503,7 +7506,7 @@
       </c>
       <c r="AE3" s="75">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF3" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7635,7 +7638,7 @@
       </c>
       <c r="AB4" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>203</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7647,7 +7650,7 @@
       </c>
       <c r="AE4" s="75">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF4" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7775,7 +7778,7 @@
       </c>
       <c r="AB5" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>444</v>
+        <v>3</v>
       </c>
       <c r="AC5" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7787,7 +7790,7 @@
       </c>
       <c r="AE5" s="75">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF5" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7915,7 +7918,7 @@
       </c>
       <c r="AB6" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>671</v>
+        <v>5</v>
       </c>
       <c r="AC6" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7927,7 +7930,7 @@
       </c>
       <c r="AE6" s="75">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF6" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8055,7 +8058,7 @@
       </c>
       <c r="AB7" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>905</v>
+        <v>7</v>
       </c>
       <c r="AC7" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -8067,7 +8070,7 @@
       </c>
       <c r="AE7" s="75">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF7" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8195,7 +8198,7 @@
       </c>
       <c r="AB8" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1176</v>
+        <v>9</v>
       </c>
       <c r="AC8" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -8207,7 +8210,7 @@
       </c>
       <c r="AE8" s="75">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>2500</v>
       </c>
       <c r="AF8" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8726,8 +8729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I7"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9133,7 +9136,10 @@
         <v>12.36679</v>
       </c>
     </row>
-    <row r="17" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
       <c r="M17" t="s">
         <v>61</v>
       </c>
@@ -9159,7 +9165,14 @@
         <v>0.45284400000000002</v>
       </c>
     </row>
-    <row r="18" spans="13:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>2.6463999999999999</v>
+      </c>
+      <c r="G18">
+        <f>F18*1000</f>
+        <v>2646.3999999999996</v>
+      </c>
       <c r="M18" s="33" t="s">
         <v>62</v>
       </c>
@@ -9185,7 +9198,14 @@
         <v>1.7726329999999999</v>
       </c>
     </row>
-    <row r="19" spans="13:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>5.7465999999999999</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19:G24" si="0">F19*1000</f>
+        <v>5746.6</v>
+      </c>
       <c r="M19" s="33" t="s">
         <v>67</v>
       </c>
@@ -9211,7 +9231,14 @@
         <v>35.461190000000002</v>
       </c>
     </row>
-    <row r="20" spans="13:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>6.742</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>6742</v>
+      </c>
       <c r="M20" s="33" t="s">
         <v>63</v>
       </c>
@@ -9237,7 +9264,14 @@
         <v>4.984934</v>
       </c>
     </row>
-    <row r="21" spans="13:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>5.0091999999999999</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>5009.2</v>
+      </c>
       <c r="M21" s="33" t="s">
         <v>64</v>
       </c>
@@ -9263,7 +9297,14 @@
         <v>4.5795250000000003</v>
       </c>
     </row>
-    <row r="22" spans="13:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>5.2344999999999997</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>5234.5</v>
+      </c>
       <c r="M22" s="33" t="s">
         <v>65</v>
       </c>
@@ -9289,7 +9330,14 @@
         <v>2.542027</v>
       </c>
     </row>
-    <row r="23" spans="13:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>5.3720999999999997</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>5372.0999999999995</v>
+      </c>
       <c r="M23" s="33" t="s">
         <v>66</v>
       </c>
@@ -9315,7 +9363,14 @@
         <v>6.3714459999999997</v>
       </c>
     </row>
-    <row r="24" spans="13:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>3.9752000000000001</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>3975.2000000000003</v>
+      </c>
       <c r="M24" s="34" t="s">
         <v>68</v>
       </c>
@@ -9341,7 +9396,11 @@
         <v>11.6691</v>
       </c>
     </row>
-    <row r="25" spans="13:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f>MIN(G18:G24)</f>
+        <v>2646.3999999999996</v>
+      </c>
       <c r="M25" s="33" t="s">
         <v>69</v>
       </c>

</xml_diff>